<commit_message>
Added more calculations for hybrid
</commit_message>
<xml_diff>
--- a/Merijumi.xlsx
+++ b/Merijumi.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bakalaurs_praktiskais\Bakalaura-darbs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFC5490-AF63-4FC7-AC9E-F80DD68BFBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5ED92CB-0C88-44F8-AFC0-47FD2CEEBBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{BF96F9AC-C4F0-49FC-AA7C-DBFC0882E122}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{BF96F9AC-C4F0-49FC-AA7C-DBFC0882E122}"/>
   </bookViews>
   <sheets>
     <sheet name="Content_based_TF_IDF" sheetId="1" r:id="rId1"/>
     <sheet name="Matrix_factorization" sheetId="2" r:id="rId2"/>
+    <sheet name="Hybrid" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="705">
   <si>
     <t>Lietotāju skaits = 10, ieteikumu skaits = 5</t>
   </si>
@@ -1930,17 +1931,240 @@
   </si>
   <si>
     <t>OVERALL        0.6630     0.8618</t>
+  </si>
+  <si>
+    <t>[{'K': 5,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Precision': 0.9340163934426233,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Recall': 0.3799638415827514,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'F1': 0.4676492468159005},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'K': 6,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Precision': 0.93379781420765,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Recall': 0.43275423000128177,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'F1': 0.5147750581164012},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'K': 7,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Precision': 0.9315729898516778,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Recall': 0.47935763476249804,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'F1': 0.553997677754133},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'K': 8,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Precision': 0.9296994535519127,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Recall': 0.519100691101128,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'F1': 0.5870314653847017},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'K': 9,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Precision': 0.9281511839708576,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Recall': 0.5533207211793922,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'F1': 0.6146836347662783},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'K': 10,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Precision': 0.9270036429872487,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Recall': 0.5827825446860294,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'F1': 0.638570847084286},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'K': 11,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Precision': 0.9261094552078167,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Recall': 0.6085515445164763,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'F1': 0.6594327548624893},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'K': 12,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Precision': 0.9259480046365299,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Recall': 0.6322367011383381,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'F1': 0.6784673740501662},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'K': 13,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Precision': 0.9257168150610772,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Recall': 0.653608646692628,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'F1': 0.6954848894426802},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'K': 14,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Precision': 0.9250502684928912,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Recall': 0.6719460120878878,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'F1': 0.7100616934583792},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'K': 15,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Precision': 0.9231064745818857,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Recall': 0.6878501775220348,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'F1': 0.7222513892076381},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'K': 16,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Precision': 0.9225258734889884,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Recall': 0.7024336594412206,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'F1': 0.733810924342122},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'K': 17,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Precision': 0.9209950152440499,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Recall': 0.7150552095275611,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'F1': 0.7435921081803183},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'K': 18,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Precision': 0.9193503136475664,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Recall': 0.726621024899465,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'F1': 0.7523662138376558},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'K': 19,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Precision': 0.9186504766233116,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Recall': 0.7380634320208769,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'F1': 0.7612079784344215},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'K': 20,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Precision': 0.9178308044921633,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'Recall': 0.7483599931539526,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'F1': 0.7691268198694231}]</t>
+  </si>
+  <si>
+    <t>Ieteikumu skaits</t>
+  </si>
+  <si>
+    <t>F1 mērījums</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>n_users</t>
+  </si>
+  <si>
+    <t>top_rec</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>n-users</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1954,16 +2178,42 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2058,11 +2308,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2084,6 +2373,19 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2453,7 +2755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE02654-32D7-4FC1-B716-6485A1C92A4B}">
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H94" sqref="H94"/>
     </sheetView>
   </sheetViews>
@@ -2468,14 +2770,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -2583,14 +2885,14 @@
       <c r="B9" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -2701,14 +3003,14 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -2819,14 +3121,14 @@
       <c r="F40" s="1"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="20" t="s">
+      <c r="A42" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
@@ -2937,14 +3239,14 @@
       <c r="F53" s="1"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="20"/>
+      <c r="B56" s="25"/>
+      <c r="C56" s="25"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="25"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
@@ -3043,7 +3345,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
       <c r="D63">
-        <f t="shared" ref="C63:D63" si="3">AVERAGE(D58:D62)</f>
+        <f t="shared" ref="D63" si="3">AVERAGE(D58:D62)</f>
         <v>8.9999999999999976E-3</v>
       </c>
     </row>
@@ -3055,14 +3357,14 @@
       <c r="F67" s="1"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="20" t="s">
+      <c r="A70" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B70" s="20"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="20"/>
+      <c r="B70" s="25"/>
+      <c r="C70" s="25"/>
+      <c r="D70" s="25"/>
+      <c r="E70" s="25"/>
+      <c r="F70" s="25"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
@@ -3173,14 +3475,14 @@
       <c r="F81" s="1"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" s="21" t="s">
+      <c r="A83" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B83" s="21"/>
-      <c r="C83" s="21"/>
-      <c r="D83" s="21"/>
-      <c r="E83" s="21"/>
-      <c r="F83" s="21"/>
+      <c r="B83" s="26"/>
+      <c r="C83" s="26"/>
+      <c r="D83" s="26"/>
+      <c r="E83" s="26"/>
+      <c r="F83" s="26"/>
     </row>
     <row r="84" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="4"/>
@@ -3201,175 +3503,175 @@
       <c r="B85" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C85" s="16">
+      <c r="C85" s="21">
         <f>B8</f>
         <v>0.1</v>
       </c>
-      <c r="D85" s="18">
+      <c r="D85" s="23">
         <f>C8</f>
         <v>3.2440000000000004E-2</v>
       </c>
-      <c r="E85" s="16">
+      <c r="E85" s="21">
         <f>D8</f>
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="F85" s="11"/>
-      <c r="G85" s="11"/>
+      <c r="F85" s="16"/>
+      <c r="G85" s="16"/>
     </row>
     <row r="86" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B86" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C86" s="17"/>
-      <c r="D86" s="19"/>
-      <c r="E86" s="17"/>
-      <c r="F86" s="11"/>
-      <c r="G86" s="11"/>
+      <c r="C86" s="22"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="16"/>
+      <c r="G86" s="16"/>
     </row>
     <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B87" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C87" s="16">
+      <c r="C87" s="21">
         <f>B22</f>
         <v>0.13800000000000001</v>
       </c>
-      <c r="D87" s="18">
+      <c r="D87" s="23">
         <f>C22</f>
         <v>2.4399999999999999E-3</v>
       </c>
-      <c r="E87" s="16">
+      <c r="E87" s="21">
         <f>D22</f>
         <v>7.7200000000000003E-3</v>
       </c>
-      <c r="F87" s="11"/>
-      <c r="G87" s="11"/>
+      <c r="F87" s="16"/>
+      <c r="G87" s="16"/>
     </row>
     <row r="88" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B88" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C88" s="17"/>
-      <c r="D88" s="19"/>
-      <c r="E88" s="17"/>
-      <c r="F88" s="11"/>
-      <c r="G88" s="11"/>
+      <c r="C88" s="22"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="22"/>
+      <c r="F88" s="16"/>
+      <c r="G88" s="16"/>
     </row>
     <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B89" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C89" s="16">
+      <c r="C89" s="21">
         <f>B36</f>
         <v>0.12640000000000001</v>
       </c>
-      <c r="D89" s="16">
+      <c r="D89" s="21">
         <f>C36</f>
         <v>1.72E-3</v>
       </c>
-      <c r="E89" s="16">
+      <c r="E89" s="21">
         <f>D36</f>
         <v>3.3799999999999998E-3</v>
       </c>
-      <c r="F89" s="11"/>
-      <c r="G89" s="11"/>
+      <c r="F89" s="16"/>
+      <c r="G89" s="16"/>
     </row>
     <row r="90" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B90" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C90" s="17"/>
-      <c r="D90" s="17"/>
-      <c r="E90" s="17"/>
-      <c r="F90" s="11"/>
-      <c r="G90" s="11"/>
+      <c r="C90" s="22"/>
+      <c r="D90" s="22"/>
+      <c r="E90" s="22"/>
+      <c r="F90" s="16"/>
+      <c r="G90" s="16"/>
     </row>
     <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B91" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C91" s="13">
+      <c r="C91" s="18">
         <f>B49</f>
         <v>0.14199999999999999</v>
       </c>
-      <c r="D91" s="13">
+      <c r="D91" s="18">
         <f>C49</f>
         <v>3.6800000000000001E-3</v>
       </c>
-      <c r="E91" s="13">
+      <c r="E91" s="18">
         <f>D49</f>
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="F91" s="12"/>
-      <c r="G91" s="12"/>
+      <c r="F91" s="17"/>
+      <c r="G91" s="17"/>
     </row>
     <row r="92" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B92" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C92" s="14"/>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="12"/>
-      <c r="G92" s="12"/>
+      <c r="C92" s="19"/>
+      <c r="D92" s="19"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="17"/>
+      <c r="G92" s="17"/>
     </row>
     <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B93" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C93" s="13">
+      <c r="C93" s="18">
         <f>B63</f>
         <v>0.13900000000000001</v>
       </c>
-      <c r="D93" s="13">
+      <c r="D93" s="18">
         <f>C63</f>
         <v>4.7000000000000002E-3</v>
       </c>
-      <c r="E93" s="13">
+      <c r="E93" s="18">
         <f>D63</f>
         <v>8.9999999999999976E-3</v>
       </c>
-      <c r="F93" s="12"/>
-      <c r="G93" s="12"/>
+      <c r="F93" s="17"/>
+      <c r="G93" s="17"/>
     </row>
     <row r="94" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B94" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C94" s="14"/>
-      <c r="D94" s="14"/>
-      <c r="E94" s="14"/>
-      <c r="F94" s="12"/>
-      <c r="G94" s="12"/>
+      <c r="C94" s="19"/>
+      <c r="D94" s="19"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="17"/>
+      <c r="G94" s="17"/>
     </row>
     <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B95" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C95" s="13">
+      <c r="C95" s="18">
         <f>B77</f>
         <v>0.1376</v>
       </c>
-      <c r="D95" s="13">
+      <c r="D95" s="18">
         <f>C77</f>
         <v>9.3600000000000003E-3</v>
       </c>
-      <c r="E95" s="13">
+      <c r="E95" s="18">
         <f>D77</f>
         <v>1.7120000000000003E-2</v>
       </c>
-      <c r="F95" s="12"/>
-      <c r="G95" s="12"/>
+      <c r="F95" s="17"/>
+      <c r="G95" s="17"/>
     </row>
     <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B96" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C96" s="15"/>
-      <c r="D96" s="15"/>
-      <c r="E96" s="15"/>
-      <c r="F96" s="12"/>
-      <c r="G96" s="12"/>
+      <c r="C96" s="20"/>
+      <c r="D96" s="20"/>
+      <c r="E96" s="20"/>
+      <c r="F96" s="17"/>
+      <c r="G96" s="17"/>
     </row>
     <row r="97" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B97" s="8" t="s">
@@ -3436,10 +3738,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0270422-7FAF-41C3-B591-4E1286951DC1}">
-  <dimension ref="B1:B613"/>
+  <dimension ref="B1:O613"/>
   <sheetViews>
-    <sheetView topLeftCell="A492" workbookViewId="0">
-      <selection activeCell="C613" sqref="A1:C613"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11:O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3447,326 +3749,657 @@
     <col min="2" max="2" width="25.88671875" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" customWidth="1"/>
+    <col min="14" max="14" width="15.88671875" customWidth="1"/>
+    <col min="15" max="15" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>631</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>695</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>632</v>
+      </c>
+      <c r="L2" s="13">
+        <v>5</v>
+      </c>
+      <c r="M2" s="14">
+        <v>0.93169999999999997</v>
+      </c>
+      <c r="N2" s="14">
+        <v>0.37990000000000002</v>
+      </c>
+      <c r="O2" s="14">
+        <v>0.46789999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>633</v>
+      </c>
+      <c r="L3" s="13">
+        <v>7</v>
+      </c>
+      <c r="M3" s="14">
+        <v>0.92830000000000001</v>
+      </c>
+      <c r="N3" s="14">
+        <v>0.47960000000000003</v>
+      </c>
+      <c r="O3" s="14">
+        <v>0.55430000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>634</v>
+      </c>
+      <c r="L4" s="13">
+        <v>9</v>
+      </c>
+      <c r="M4" s="14">
+        <v>0.92549999999999999</v>
+      </c>
+      <c r="N4" s="14">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="O4" s="14">
+        <v>0.61480000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>635</v>
+      </c>
+      <c r="L5" s="13">
+        <v>11</v>
+      </c>
+      <c r="M5" s="14">
+        <v>0.92120000000000002</v>
+      </c>
+      <c r="N5" s="14">
+        <v>0.60750000000000004</v>
+      </c>
+      <c r="O5" s="14">
+        <v>0.65900000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>636</v>
+      </c>
+      <c r="L6" s="13">
+        <v>13</v>
+      </c>
+      <c r="M6" s="14">
+        <v>0.91739999999999999</v>
+      </c>
+      <c r="N6" s="14">
+        <v>0.64949999999999997</v>
+      </c>
+      <c r="O6" s="14">
+        <v>0.69220000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>637</v>
+      </c>
+      <c r="L7" s="13">
+        <v>15</v>
+      </c>
+      <c r="M7" s="14">
+        <v>0.91590000000000005</v>
+      </c>
+      <c r="N7" s="14">
+        <v>0.68359999999999999</v>
+      </c>
+      <c r="O7" s="14">
+        <v>0.71930000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>638</v>
+      </c>
+      <c r="L8" s="13">
+        <v>17</v>
+      </c>
+      <c r="M8" s="14">
+        <v>0.91510000000000002</v>
+      </c>
+      <c r="N8" s="14">
+        <v>0.7127</v>
+      </c>
+      <c r="O8" s="14">
+        <v>0.74209999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>639</v>
+      </c>
+      <c r="L9" s="13">
+        <v>19</v>
+      </c>
+      <c r="M9" s="14">
+        <v>0.91339999999999999</v>
+      </c>
+      <c r="N9" s="14">
+        <v>0.73640000000000005</v>
+      </c>
+      <c r="O9" s="14">
+        <v>0.76049999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>640</v>
+      </c>
+      <c r="L10" s="13">
+        <v>20</v>
+      </c>
+      <c r="M10" s="14">
+        <v>0.91210000000000002</v>
+      </c>
+      <c r="N10" s="14">
+        <v>0.74639999999999995</v>
+      </c>
+      <c r="O10" s="14">
+        <v>0.76800000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>641</v>
+      </c>
+      <c r="L11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M11" s="15">
+        <f>AVERAGE(M2:M10)</f>
+        <v>0.92006666666666659</v>
+      </c>
+      <c r="N11" s="15">
+        <f t="shared" ref="N11:O11" si="0">AVERAGE(N2:N10)</f>
+        <v>0.61639999999999995</v>
+      </c>
+      <c r="O11" s="15">
+        <f t="shared" si="0"/>
+        <v>0.66423333333333334</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F26" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F28" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F32" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F34" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F35" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F36" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F37" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F38" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F39" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F40" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F42" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F43" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F44" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F45" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F46" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F47" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F48" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F49" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F50" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F51" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F52" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F53" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F54" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F55" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F56" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F57" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F58" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F59" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F60" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F61" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F62" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="F63" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>81</v>
+      </c>
+      <c r="F64" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.3">
@@ -6512,6 +7145,429 @@
     <row r="613" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B613" t="s">
         <v>630</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482949DF-3F24-4337-BE7A-CD50A5519C08}">
+  <dimension ref="A1:P21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>697</v>
+      </c>
+      <c r="C1" t="s">
+        <v>698</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>699</v>
+      </c>
+      <c r="F1" t="s">
+        <v>700</v>
+      </c>
+      <c r="G1" t="s">
+        <v>701</v>
+      </c>
+      <c r="H1" t="s">
+        <v>702</v>
+      </c>
+      <c r="J1" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.4</v>
+      </c>
+      <c r="C2">
+        <v>1.7100000000000001E-2</v>
+      </c>
+      <c r="D2">
+        <v>3.2800000000000003E-2</v>
+      </c>
+      <c r="E2">
+        <v>0.64139999999999997</v>
+      </c>
+      <c r="F2">
+        <v>0.78390000000000004</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C3">
+        <v>1.55E-2</v>
+      </c>
+      <c r="D3">
+        <v>2.92E-2</v>
+      </c>
+      <c r="E3">
+        <v>0.84060000000000001</v>
+      </c>
+      <c r="F3">
+        <v>1.0117</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.22</v>
+      </c>
+      <c r="C4">
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="D4">
+        <v>2.47E-2</v>
+      </c>
+      <c r="E4">
+        <v>0.78549999999999998</v>
+      </c>
+      <c r="F4">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.2</v>
+      </c>
+      <c r="C5">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.0299999999999999E-2</v>
+      </c>
+      <c r="E5">
+        <v>0.80789999999999995</v>
+      </c>
+      <c r="F5">
+        <v>0.97619999999999996</v>
+      </c>
+      <c r="G5">
+        <v>50</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.26</v>
+      </c>
+      <c r="C6">
+        <v>3.73E-2</v>
+      </c>
+      <c r="D6">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.6865</v>
+      </c>
+      <c r="F6">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.26</v>
+      </c>
+      <c r="C7">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="D7">
+        <v>5.8099999999999999E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.75739999999999996</v>
+      </c>
+      <c r="F7">
+        <v>0.91659999999999997</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.23</v>
+      </c>
+      <c r="C8">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="D8">
+        <v>3.9100000000000003E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.8246</v>
+      </c>
+      <c r="F8">
+        <v>0.98319999999999996</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.2</v>
+      </c>
+      <c r="C9">
+        <v>3.4200000000000001E-2</v>
+      </c>
+      <c r="D9">
+        <v>5.6899999999999999E-2</v>
+      </c>
+      <c r="E9">
+        <v>0.83309999999999995</v>
+      </c>
+      <c r="F9">
+        <v>0.98650000000000004</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.22</v>
+      </c>
+      <c r="C10">
+        <v>3.7199999999999997E-2</v>
+      </c>
+      <c r="D10">
+        <v>5.9799999999999999E-2</v>
+      </c>
+      <c r="E10">
+        <v>0.8085</v>
+      </c>
+      <c r="F10">
+        <v>0.96589999999999998</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0.17249999999999999</v>
+      </c>
+      <c r="C11">
+        <v>3.15E-2</v>
+      </c>
+      <c r="D11">
+        <v>5.04E-2</v>
+      </c>
+      <c r="E11">
+        <v>0.81720000000000004</v>
+      </c>
+      <c r="F11">
+        <v>0.98360000000000003</v>
+      </c>
+      <c r="G11">
+        <v>20</v>
+      </c>
+      <c r="H11">
+        <v>20</v>
+      </c>
+      <c r="O11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <f>AVERAGE(B2:B11)</f>
+        <v>0.24425000000000002</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:D13" si="0">AVERAGE(C2:C11)</f>
+        <v>2.5170000000000005E-2</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>4.3630000000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <f>AVERAGE(B2:B9)</f>
+        <v>0.25625000000000003</v>
+      </c>
+      <c r="C14">
+        <f>AVERAGE(C2:C9)</f>
+        <v>2.2875000000000003E-2</v>
+      </c>
+      <c r="D14">
+        <f>AVERAGE(D2:D9)</f>
+        <v>4.07625E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="M18" t="s">
+        <v>703</v>
+      </c>
+      <c r="O18" t="s">
+        <v>704</v>
+      </c>
+      <c r="P18" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="19" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>0.16</v>
+      </c>
+      <c r="H19">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="I19">
+        <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="J19">
+        <v>0.77229999999999999</v>
+      </c>
+      <c r="K19">
+        <v>0.9375</v>
+      </c>
+      <c r="M19">
+        <v>50</v>
+      </c>
+      <c r="O19">
+        <v>5</v>
+      </c>
+      <c r="P19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>0.4</v>
+      </c>
+      <c r="H20">
+        <v>1.7100000000000001E-2</v>
+      </c>
+      <c r="I20">
+        <v>3.2800000000000003E-2</v>
+      </c>
+      <c r="J20">
+        <v>0.64139999999999997</v>
+      </c>
+      <c r="K20">
+        <v>0.78390000000000004</v>
+      </c>
+      <c r="M20">
+        <v>60</v>
+      </c>
+      <c r="O20">
+        <v>5</v>
+      </c>
+      <c r="P20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="M21">
+        <v>70</v>
+      </c>
+      <c r="O21">
+        <v>5</v>
+      </c>
+      <c r="P21">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>